<commit_message>
Added antenna to BOM
</commit_message>
<xml_diff>
--- a/CHECON.BOM.xlsx
+++ b/CHECON.BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="83">
   <si>
     <t>Product Name:</t>
   </si>
@@ -246,6 +246,21 @@
   </si>
   <si>
     <t>http://www.mcmaster.com/#94812a200/=vrk1cp</t>
+  </si>
+  <si>
+    <t>Antenna</t>
+  </si>
+  <si>
+    <t>2.4Ghz swivel antenna for wireless connectivity</t>
+  </si>
+  <si>
+    <t>S181FL-5-RMM-2450S</t>
+  </si>
+  <si>
+    <t>Qwiksource</t>
+  </si>
+  <si>
+    <t>http://qwiksource.com/</t>
   </si>
   <si>
     <t>     </t>
@@ -259,7 +274,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -352,6 +367,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -407,7 +428,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -498,6 +519,10 @@
     </xf>
     <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -580,9 +605,9 @@
   <dimension ref="A1:Q75"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="36:36"/>
+      <selection pane="bottomLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -745,6 +770,8 @@
       <c r="H6" s="11"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
+      <c r="K6" s="0"/>
+      <c r="L6" s="0"/>
       <c r="O6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -758,6 +785,8 @@
       <c r="H7" s="11"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
+      <c r="K7" s="0"/>
+      <c r="L7" s="0"/>
       <c r="O7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -771,6 +800,8 @@
       <c r="H8" s="11"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
       <c r="O8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -796,6 +827,8 @@
       <c r="H9" s="15"/>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
+      <c r="K9" s="0"/>
+      <c r="L9" s="0"/>
       <c r="O9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -809,6 +842,8 @@
       <c r="H10" s="11"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
+      <c r="K10" s="0"/>
+      <c r="L10" s="0"/>
       <c r="O10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -834,6 +869,8 @@
       <c r="H11" s="11"/>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
+      <c r="K11" s="0"/>
+      <c r="L11" s="0"/>
       <c r="O11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -847,6 +884,8 @@
       <c r="H12" s="11"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
+      <c r="K12" s="0"/>
+      <c r="L12" s="0"/>
       <c r="O12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -872,6 +911,8 @@
       <c r="H13" s="11"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
+      <c r="K13" s="0"/>
+      <c r="L13" s="0"/>
       <c r="O13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -885,6 +926,8 @@
       <c r="H14" s="11"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
+      <c r="K14" s="0"/>
+      <c r="L14" s="0"/>
       <c r="O14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -910,6 +953,8 @@
       <c r="H15" s="15"/>
       <c r="I15" s="17"/>
       <c r="J15" s="12"/>
+      <c r="K15" s="0"/>
+      <c r="L15" s="0"/>
       <c r="O15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -923,6 +968,8 @@
       <c r="H16" s="11"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
+      <c r="K16" s="0"/>
+      <c r="L16" s="0"/>
       <c r="O16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -946,6 +993,8 @@
       <c r="H17" s="11"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
+      <c r="K17" s="0"/>
+      <c r="L17" s="0"/>
       <c r="O17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -959,6 +1008,8 @@
       <c r="H18" s="11"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
+      <c r="K18" s="0"/>
+      <c r="L18" s="0"/>
       <c r="O18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -982,6 +1033,8 @@
       <c r="H19" s="11"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
+      <c r="K19" s="0"/>
+      <c r="L19" s="0"/>
       <c r="O19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -995,6 +1048,8 @@
       <c r="H20" s="11"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
+      <c r="K20" s="0"/>
+      <c r="L20" s="0"/>
       <c r="O20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1020,6 +1075,8 @@
       <c r="H21" s="11"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
+      <c r="K21" s="0"/>
+      <c r="L21" s="0"/>
       <c r="O21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1033,6 +1090,8 @@
       <c r="H22" s="11"/>
       <c r="I22" s="13"/>
       <c r="J22" s="12"/>
+      <c r="K22" s="0"/>
+      <c r="L22" s="0"/>
       <c r="O22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1058,6 +1117,8 @@
       <c r="H23" s="11"/>
       <c r="I23" s="13"/>
       <c r="J23" s="12"/>
+      <c r="K23" s="0"/>
+      <c r="L23" s="0"/>
       <c r="O23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1071,6 +1132,8 @@
       <c r="H24" s="11"/>
       <c r="I24" s="13"/>
       <c r="J24" s="12"/>
+      <c r="K24" s="0"/>
+      <c r="L24" s="0"/>
       <c r="O24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1096,6 +1159,8 @@
       <c r="H25" s="11"/>
       <c r="I25" s="13"/>
       <c r="J25" s="12"/>
+      <c r="K25" s="0"/>
+      <c r="L25" s="0"/>
       <c r="O25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1109,6 +1174,8 @@
       <c r="H26" s="11"/>
       <c r="I26" s="13"/>
       <c r="J26" s="12"/>
+      <c r="K26" s="0"/>
+      <c r="L26" s="0"/>
       <c r="O26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1134,6 +1201,8 @@
       </c>
       <c r="I27" s="13"/>
       <c r="J27" s="12"/>
+      <c r="K27" s="0"/>
+      <c r="L27" s="0"/>
       <c r="O27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1147,6 +1216,8 @@
       <c r="H28" s="11"/>
       <c r="I28" s="13"/>
       <c r="J28" s="12"/>
+      <c r="K28" s="0"/>
+      <c r="L28" s="0"/>
       <c r="O28" s="13"/>
     </row>
     <row r="29" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1172,6 +1243,8 @@
       </c>
       <c r="I29" s="13"/>
       <c r="J29" s="12"/>
+      <c r="K29" s="0"/>
+      <c r="L29" s="0"/>
       <c r="O29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1185,6 +1258,8 @@
       <c r="H30" s="11"/>
       <c r="I30" s="13"/>
       <c r="J30" s="12"/>
+      <c r="K30" s="0"/>
+      <c r="L30" s="0"/>
       <c r="O30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1210,6 +1285,8 @@
       </c>
       <c r="I31" s="13"/>
       <c r="J31" s="12"/>
+      <c r="K31" s="0"/>
+      <c r="L31" s="0"/>
       <c r="O31" s="13"/>
     </row>
     <row r="32" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1223,6 +1300,8 @@
       <c r="H32" s="11"/>
       <c r="I32" s="13"/>
       <c r="J32" s="12"/>
+      <c r="K32" s="0"/>
+      <c r="L32" s="0"/>
       <c r="O32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1248,6 +1327,8 @@
       </c>
       <c r="I33" s="13"/>
       <c r="J33" s="12"/>
+      <c r="K33" s="0"/>
+      <c r="L33" s="0"/>
       <c r="O33" s="13"/>
     </row>
     <row r="34" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1261,6 +1342,8 @@
       <c r="H34" s="11"/>
       <c r="I34" s="13"/>
       <c r="J34" s="12"/>
+      <c r="K34" s="0"/>
+      <c r="L34" s="0"/>
       <c r="O34" s="13"/>
     </row>
     <row r="35" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1286,6 +1369,8 @@
       </c>
       <c r="I35" s="13"/>
       <c r="J35" s="12"/>
+      <c r="K35" s="0"/>
+      <c r="L35" s="0"/>
       <c r="O35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1299,6 +1384,8 @@
       <c r="H36" s="11"/>
       <c r="I36" s="13"/>
       <c r="J36" s="12"/>
+      <c r="K36" s="0"/>
+      <c r="L36" s="0"/>
       <c r="O36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1324,6 +1411,8 @@
       </c>
       <c r="I37" s="13"/>
       <c r="J37" s="12"/>
+      <c r="K37" s="0"/>
+      <c r="L37" s="0"/>
       <c r="O37" s="13"/>
     </row>
     <row r="38" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1337,19 +1426,35 @@
       <c r="H38" s="11"/>
       <c r="I38" s="13"/>
       <c r="J38" s="12"/>
+      <c r="K38" s="0"/>
+      <c r="L38" s="0"/>
       <c r="O38" s="13"/>
     </row>
     <row r="39" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
+      <c r="A39" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>79</v>
+      </c>
       <c r="E39" s="15"/>
       <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
+      <c r="G39" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>81</v>
+      </c>
       <c r="I39" s="13"/>
       <c r="J39" s="12"/>
+      <c r="K39" s="0"/>
+      <c r="L39" s="0"/>
       <c r="O39" s="13"/>
     </row>
     <row r="40" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1363,6 +1468,8 @@
       <c r="H40" s="11"/>
       <c r="I40" s="13"/>
       <c r="J40" s="12"/>
+      <c r="K40" s="0"/>
+      <c r="L40" s="0"/>
       <c r="O40" s="13"/>
     </row>
     <row r="41" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1376,6 +1483,8 @@
       <c r="H41" s="11"/>
       <c r="I41" s="13"/>
       <c r="J41" s="12"/>
+      <c r="K41" s="0"/>
+      <c r="L41" s="0"/>
       <c r="O41" s="13"/>
     </row>
     <row r="42" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1389,6 +1498,8 @@
       <c r="H42" s="11"/>
       <c r="I42" s="13"/>
       <c r="J42" s="12"/>
+      <c r="K42" s="0"/>
+      <c r="L42" s="0"/>
       <c r="O42" s="13"/>
     </row>
     <row r="43" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1402,6 +1513,8 @@
       <c r="H43" s="11"/>
       <c r="I43" s="13"/>
       <c r="J43" s="12"/>
+      <c r="K43" s="0"/>
+      <c r="L43" s="0"/>
       <c r="O43" s="13"/>
     </row>
     <row r="44" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1415,6 +1528,8 @@
       <c r="H44" s="11"/>
       <c r="I44" s="13"/>
       <c r="J44" s="12"/>
+      <c r="K44" s="0"/>
+      <c r="L44" s="0"/>
       <c r="O44" s="13"/>
     </row>
     <row r="45" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1428,6 +1543,8 @@
       <c r="H45" s="11"/>
       <c r="I45" s="13"/>
       <c r="J45" s="12"/>
+      <c r="K45" s="0"/>
+      <c r="L45" s="0"/>
       <c r="O45" s="13"/>
     </row>
     <row r="46" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1441,6 +1558,8 @@
       <c r="H46" s="15"/>
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
+      <c r="K46" s="0"/>
+      <c r="L46" s="0"/>
       <c r="O46" s="13"/>
     </row>
     <row r="47" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1454,6 +1573,8 @@
       <c r="H47" s="15"/>
       <c r="I47" s="17"/>
       <c r="J47" s="12"/>
+      <c r="K47" s="0"/>
+      <c r="L47" s="0"/>
       <c r="O47" s="13"/>
     </row>
     <row r="48" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1467,6 +1588,8 @@
       <c r="H48" s="15"/>
       <c r="I48" s="17"/>
       <c r="J48" s="12"/>
+      <c r="K48" s="0"/>
+      <c r="L48" s="0"/>
       <c r="O48" s="13"/>
     </row>
     <row r="49" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1480,6 +1603,8 @@
       <c r="H49" s="15"/>
       <c r="I49" s="17"/>
       <c r="J49" s="12"/>
+      <c r="K49" s="0"/>
+      <c r="L49" s="0"/>
       <c r="O49" s="13"/>
     </row>
     <row r="50" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1493,6 +1618,8 @@
       <c r="H50" s="15"/>
       <c r="I50" s="17"/>
       <c r="J50" s="12"/>
+      <c r="K50" s="0"/>
+      <c r="L50" s="0"/>
       <c r="O50" s="13"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1515,7 +1642,7 @@
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>
       <c r="D52" s="11" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E52" s="11"/>
       <c r="F52" s="11"/>
@@ -1527,7 +1654,6 @@
       <c r="L52" s="12"/>
       <c r="O52" s="13"/>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1539,6 +1665,7 @@
     <hyperlink ref="H33" r:id="rId4" display="http://www.digikey.com/product-detail/en/VLP-400-F/492-1516-ND/3101279"/>
     <hyperlink ref="H35" r:id="rId5" display="http://www.mouser.com/ProductDetail/Bivar/9908-3MM/?qs=sGAEpiMZZMtrde5aJd3qw%252bna4uFHzhhu0MrroqtKyos%3d"/>
     <hyperlink ref="H37" r:id="rId6" location="94812a200/=vrk1cp" display="http://www.mcmaster.com/#94812a200/=vrk1cp"/>
+    <hyperlink ref="H39" r:id="rId7" display="http://qwiksource.com/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Changed drawing names to reflect new versions
</commit_message>
<xml_diff>
--- a/CHECON.BOM.xlsx
+++ b/CHECON.BOM.xlsx
@@ -73,34 +73,34 @@
     <t>CHECON.FACE</t>
   </si>
   <si>
+    <t>VER 1.1 REV B</t>
+  </si>
+  <si>
+    <t>Mean Machine Inc.</t>
+  </si>
+  <si>
+    <t>Screen Coverplate Top</t>
+  </si>
+  <si>
+    <t>Lasercut Acrylic Screen Cover</t>
+  </si>
+  <si>
+    <t>CHECON.COVER</t>
+  </si>
+  <si>
+    <t>Ponoko</t>
+  </si>
+  <si>
+    <t>Screen Coverplate Bottom</t>
+  </si>
+  <si>
+    <t>Lasercut Acrylic Screen alignment tray</t>
+  </si>
+  <si>
+    <t>CHECON.TRAY</t>
+  </si>
+  <si>
     <t>VER 1.0 REV A</t>
-  </si>
-  <si>
-    <t>Mean Machine Inc.</t>
-  </si>
-  <si>
-    <t>Screen Coverplate Top</t>
-  </si>
-  <si>
-    <t>Lasercut Acrylic Screen Cover</t>
-  </si>
-  <si>
-    <t>CHECON.COVER</t>
-  </si>
-  <si>
-    <t>VER 1.1 REV B</t>
-  </si>
-  <si>
-    <t>Ponoko</t>
-  </si>
-  <si>
-    <t>Screen Coverplate Bottom</t>
-  </si>
-  <si>
-    <t>Lasercut Acrylic Screen alignment tray</t>
-  </si>
-  <si>
-    <t>CHECON.TRAY</t>
   </si>
   <si>
     <t>Zero Screw Core</t>
@@ -2027,7 +2027,7 @@
     <col min="5" max="5" width="17.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.125" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="43.4297" style="1" customWidth="1"/>
+    <col min="8" max="8" width="43.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="99.125" style="1" customWidth="1"/>
     <col min="10" max="10" width="10.125" style="1" customWidth="1"/>
     <col min="11" max="11" width="10.125" style="1" customWidth="1"/>
@@ -2261,11 +2261,11 @@
         <v>24</v>
       </c>
       <c r="E11" t="s" s="24">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F11" s="19"/>
       <c r="G11" t="s" s="23">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" s="19"/>
       <c r="I11" s="21"/>
@@ -2296,20 +2296,20 @@
         <v>1</v>
       </c>
       <c r="B13" t="s" s="24">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s" s="24">
         <v>27</v>
       </c>
-      <c r="C13" t="s" s="24">
+      <c r="D13" t="s" s="23">
         <v>28</v>
       </c>
-      <c r="D13" t="s" s="23">
+      <c r="E13" t="s" s="24">
         <v>29</v>
-      </c>
-      <c r="E13" t="s" s="24">
-        <v>20</v>
       </c>
       <c r="F13" s="19"/>
       <c r="G13" t="s" s="23">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H13" s="19"/>
       <c r="I13" s="21"/>
@@ -2349,7 +2349,7 @@
         <v>32</v>
       </c>
       <c r="E15" t="s" s="24">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F15" s="19"/>
       <c r="G15" t="s" s="24">
@@ -2477,7 +2477,7 @@
         <v>43</v>
       </c>
       <c r="E21" t="s" s="24">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" t="s" s="24">
@@ -2521,7 +2521,7 @@
         <v>46</v>
       </c>
       <c r="E23" t="s" s="24">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F23" s="19"/>
       <c r="G23" t="s" s="24">

</xml_diff>

<commit_message>
Update to BOM - removed mechanicals, added those to *.MECH BOM
</commit_message>
<xml_diff>
--- a/CHECON.BOM.xlsx
+++ b/CHECON.BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
   <si>
     <t>Product Name:</t>
   </si>
@@ -22,7 +22,7 @@
     <t>Tag:</t>
   </si>
   <si>
-    <t>CHECON.v1.1</t>
+    <t>CHECON.v1.0</t>
   </si>
   <si>
     <t>Product Number:</t>
@@ -64,52 +64,13 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Top Coverplate</t>
-  </si>
-  <si>
-    <t>Machined Aluminum Part</t>
-  </si>
-  <si>
-    <t>CHECON.FACE</t>
-  </si>
-  <si>
-    <t>VER 1.1 REV B</t>
-  </si>
-  <si>
-    <t>Mean Machine Inc.</t>
-  </si>
-  <si>
-    <t>Screen Coverplate Top</t>
-  </si>
-  <si>
-    <t>Lasercut Acrylic Screen Cover</t>
-  </si>
-  <si>
-    <t>CHECON.COVER</t>
-  </si>
-  <si>
-    <t>Ponoko</t>
-  </si>
-  <si>
-    <t>Screen Coverplate Bottom</t>
-  </si>
-  <si>
-    <t>Lasercut Acrylic Screen alignment tray</t>
-  </si>
-  <si>
-    <t>CHECON.TRAY</t>
-  </si>
-  <si>
-    <t>VER 1.0 REV A</t>
-  </si>
-  <si>
-    <t>Zero Screw Core</t>
-  </si>
-  <si>
-    <t>Lasercut and/or Machined Delrin Part</t>
-  </si>
-  <si>
-    <t>CHECON.CORETOP</t>
+    <t>CHECON.MECH</t>
+  </si>
+  <si>
+    <t>Housing Components</t>
+  </si>
+  <si>
+    <t>CHECON.MECH.v1.3</t>
   </si>
   <si>
     <t>Daughterboard PCB Assembly</t>
@@ -118,10 +79,10 @@
     <t>Daughterboard PCB</t>
   </si>
   <si>
-    <t>CHECON.PCB</t>
-  </si>
-  <si>
-    <t>CHECON.PCB.v1.0</t>
+    <t>LEDCON.PCB</t>
+  </si>
+  <si>
+    <t>LEDCON.PCB.v1.0</t>
   </si>
   <si>
     <t>KW2 PCB Assembly</t>
@@ -134,33 +95,6 @@
   </si>
   <si>
     <t>KW2CPU.PCB.v1.2</t>
-  </si>
-  <si>
-    <t>Four Screw Core B</t>
-  </si>
-  <si>
-    <t>Delrin Shell Part, Top</t>
-  </si>
-  <si>
-    <t>CHECON.COREMID</t>
-  </si>
-  <si>
-    <t>Four Screw Core A</t>
-  </si>
-  <si>
-    <t>Delrin Shell Part, Bottom</t>
-  </si>
-  <si>
-    <t>CHECON.COREBOT</t>
-  </si>
-  <si>
-    <t>Backplate</t>
-  </si>
-  <si>
-    <t>Lasercut 5052 1/16" Aluminum Sheet</t>
-  </si>
-  <si>
-    <t>CHECON.BACK</t>
   </si>
   <si>
     <t>Header Access Plug</t>
@@ -347,8 +281,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -392,17 +327,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="11"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="12"/>
-      <color indexed="12"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <u val="single"/>
       <sz val="13"/>
       <color indexed="8"/>
@@ -412,6 +336,17 @@
       <sz val="13"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color indexed="13"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -531,37 +466,37 @@
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -570,7 +505,7 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
@@ -582,7 +517,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
@@ -600,13 +535,13 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -618,7 +553,7 @@
         <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -631,7 +566,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -665,15 +600,18 @@
     <xf numFmtId="1" fontId="5" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="59" fontId="5" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
@@ -704,21 +642,21 @@
     <xf numFmtId="0" fontId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="8" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -728,10 +666,10 @@
     <xf numFmtId="1" fontId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="9" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="9" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -761,8 +699,11 @@
     <xf numFmtId="1" fontId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="8" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="10" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -783,9 +724,9 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffefefef"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffcccccc"/>
       <rgbColor rgb="ff333333"/>
       <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffcccccc"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -2014,7 +1955,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2074,7 +2015,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="11">
-        <v>42010</v>
+        <v>42129</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
@@ -2094,7 +2035,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="11">
-        <v>42107</v>
+        <v>42129</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
@@ -2110,8 +2051,8 @@
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
@@ -2122,25 +2063,25 @@
       <c r="N4" s="13"/>
     </row>
     <row r="5" ht="18" customHeight="1">
-      <c r="A5" t="s" s="14">
+      <c r="A5" t="s" s="15">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="15">
+      <c r="B5" t="s" s="16">
         <v>9</v>
       </c>
-      <c r="C5" t="s" s="15">
+      <c r="C5" t="s" s="16">
         <v>10</v>
       </c>
-      <c r="D5" t="s" s="15">
+      <c r="D5" t="s" s="16">
         <v>11</v>
       </c>
-      <c r="E5" t="s" s="15">
+      <c r="E5" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="F5" t="s" s="15">
+      <c r="F5" t="s" s="16">
         <v>13</v>
       </c>
-      <c r="G5" t="s" s="15">
+      <c r="G5" t="s" s="16">
         <v>14</v>
       </c>
       <c r="H5" t="s" s="8">
@@ -2149,987 +2090,705 @@
       <c r="I5" t="s" s="8">
         <v>16</v>
       </c>
-      <c r="J5" s="11"/>
+      <c r="J5" s="14"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
       <c r="N5" s="13"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
+      <c r="A8" s="20">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s" s="24">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s" s="24">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s" s="24">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s" s="24">
+        <v>19</v>
+      </c>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="20">
+      <c r="A9" s="21"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="21">
         <v>1</v>
       </c>
-      <c r="B9" t="s" s="23">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s" s="24">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s" s="23">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s" s="24">
+      <c r="B10" t="s" s="27">
         <v>20</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" t="s" s="24">
+      <c r="C10" t="s" s="27">
         <v>21</v>
       </c>
-      <c r="H9" s="20"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
+      <c r="D10" t="s" s="24">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s" s="27">
+        <v>23</v>
+      </c>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="19">
+      <c r="A11" s="20"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="20">
         <v>1</v>
       </c>
-      <c r="B11" t="s" s="23">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s" s="23">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s" s="23">
+      <c r="B12" t="s" s="24">
         <v>24</v>
       </c>
-      <c r="E11" t="s" s="24">
-        <v>20</v>
-      </c>
-      <c r="F11" s="19"/>
-      <c r="G11" t="s" s="23">
+      <c r="C12" t="s" s="24">
         <v>25</v>
       </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
+      <c r="D12" t="s" s="24">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s" s="27">
+        <v>27</v>
+      </c>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="20">
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+    </row>
+    <row r="14" ht="30" customHeight="1">
+      <c r="A14" s="21">
         <v>1</v>
       </c>
-      <c r="B13" t="s" s="24">
-        <v>26</v>
-      </c>
-      <c r="C13" t="s" s="24">
-        <v>27</v>
-      </c>
-      <c r="D13" t="s" s="23">
+      <c r="B14" t="s" s="27">
         <v>28</v>
       </c>
-      <c r="E13" t="s" s="24">
+      <c r="C14" t="s" s="27">
         <v>29</v>
       </c>
-      <c r="F13" s="19"/>
-      <c r="G13" t="s" s="23">
-        <v>25</v>
-      </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
+      <c r="D14" t="s" s="27">
+        <v>30</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="20"/>
+      <c r="G14" t="s" s="24">
+        <v>31</v>
+      </c>
+      <c r="H14" t="s" s="28">
+        <v>32</v>
+      </c>
+      <c r="I14" s="29"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
     </row>
     <row r="15" ht="30" customHeight="1">
-      <c r="A15" s="20">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+    </row>
+    <row r="16" ht="27" customHeight="1">
+      <c r="A16" s="21">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s" s="27">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s" s="30">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s" s="27">
+        <v>35</v>
+      </c>
+      <c r="E16" s="21"/>
+      <c r="F16" s="20"/>
+      <c r="G16" t="s" s="24">
+        <v>36</v>
+      </c>
+      <c r="H16" t="s" s="28">
+        <v>37</v>
+      </c>
+      <c r="I16" s="29"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+    </row>
+    <row r="17" ht="27" customHeight="1">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+    </row>
+    <row r="18" ht="27" customHeight="1">
+      <c r="A18" s="21">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s" s="27">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s" s="30">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s" s="27">
+        <v>40</v>
+      </c>
+      <c r="E18" s="21"/>
+      <c r="F18" s="20"/>
+      <c r="G18" t="s" s="24">
+        <v>36</v>
+      </c>
+      <c r="H18" t="s" s="28">
+        <v>41</v>
+      </c>
+      <c r="I18" s="29"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+    </row>
+    <row r="19" ht="27" customHeight="1">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+    </row>
+    <row r="20" ht="27" customHeight="1">
+      <c r="A20" s="21">
         <v>1</v>
       </c>
-      <c r="B15" t="s" s="24">
-        <v>30</v>
-      </c>
-      <c r="C15" t="s" s="24">
-        <v>31</v>
-      </c>
-      <c r="D15" t="s" s="26">
-        <v>32</v>
-      </c>
-      <c r="E15" t="s" s="24">
-        <v>29</v>
-      </c>
-      <c r="F15" s="19"/>
-      <c r="G15" t="s" s="24">
-        <v>21</v>
-      </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="20">
+      <c r="B20" t="s" s="27">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s" s="27">
+        <v>43</v>
+      </c>
+      <c r="D20" t="s" s="27">
+        <v>44</v>
+      </c>
+      <c r="E20" s="21"/>
+      <c r="F20" s="20"/>
+      <c r="G20" t="s" s="24">
+        <v>45</v>
+      </c>
+      <c r="H20" t="s" s="28">
+        <v>46</v>
+      </c>
+      <c r="I20" s="29"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+    </row>
+    <row r="21" ht="27" customHeight="1">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+    </row>
+    <row r="22" ht="27" customHeight="1">
+      <c r="A22" s="21">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s" s="27">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s" s="27">
+        <v>48</v>
+      </c>
+      <c r="D22" t="s" s="27">
+        <v>49</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="20"/>
+      <c r="G22" t="s" s="24">
+        <v>45</v>
+      </c>
+      <c r="H22" t="s" s="24">
+        <v>50</v>
+      </c>
+      <c r="I22" s="29"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+    </row>
+    <row r="23" ht="27" customHeight="1">
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+    </row>
+    <row r="24" ht="27" customHeight="1">
+      <c r="A24" s="21">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s" s="27">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s" s="27">
+        <v>52</v>
+      </c>
+      <c r="D24" t="s" s="27">
+        <v>53</v>
+      </c>
+      <c r="E24" s="21"/>
+      <c r="F24" s="20"/>
+      <c r="G24" t="s" s="24">
+        <v>36</v>
+      </c>
+      <c r="H24" t="s" s="24">
+        <v>54</v>
+      </c>
+      <c r="I24" s="29"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+    </row>
+    <row r="25" ht="27" customHeight="1">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+    </row>
+    <row r="26" ht="27" customHeight="1">
+      <c r="A26" s="21">
         <v>1</v>
       </c>
-      <c r="B17" t="s" s="24">
-        <v>33</v>
-      </c>
-      <c r="C17" t="s" s="24">
-        <v>34</v>
-      </c>
-      <c r="D17" t="s" s="23">
-        <v>35</v>
-      </c>
-      <c r="E17" t="s" s="24">
-        <v>36</v>
-      </c>
-      <c r="F17" s="19"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="19">
+      <c r="B26" t="s" s="27">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s" s="27">
+        <v>56</v>
+      </c>
+      <c r="D26" t="s" s="27">
+        <v>57</v>
+      </c>
+      <c r="E26" s="21"/>
+      <c r="F26" s="20"/>
+      <c r="G26" t="s" s="24">
+        <v>58</v>
+      </c>
+      <c r="H26" t="s" s="24">
+        <v>59</v>
+      </c>
+      <c r="I26" s="29"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+    </row>
+    <row r="27" ht="27" customHeight="1">
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+    </row>
+    <row r="28" ht="27" customHeight="1">
+      <c r="A28" s="33">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s" s="34">
+        <v>60</v>
+      </c>
+      <c r="C28" t="s" s="35">
+        <v>61</v>
+      </c>
+      <c r="D28" t="s" s="33">
+        <v>62</v>
+      </c>
+      <c r="E28" s="36"/>
+      <c r="F28" s="20"/>
+      <c r="G28" t="s" s="24">
+        <v>63</v>
+      </c>
+      <c r="H28" t="s" s="37">
+        <v>64</v>
+      </c>
+      <c r="I28" s="38"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+    </row>
+    <row r="29" ht="27" customHeight="1">
+      <c r="A29" s="39"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+    </row>
+    <row r="30" ht="27" customHeight="1">
+      <c r="A30" s="33">
         <v>1</v>
       </c>
-      <c r="B19" t="s" s="23">
-        <v>37</v>
-      </c>
-      <c r="C19" t="s" s="23">
-        <v>38</v>
-      </c>
-      <c r="D19" t="s" s="23">
-        <v>39</v>
-      </c>
-      <c r="E19" t="s" s="24">
-        <v>40</v>
-      </c>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="19">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s" s="23">
-        <v>41</v>
-      </c>
-      <c r="C21" t="s" s="23">
-        <v>42</v>
-      </c>
-      <c r="D21" t="s" s="23">
-        <v>43</v>
-      </c>
-      <c r="E21" t="s" s="24">
-        <v>29</v>
-      </c>
-      <c r="F21" s="19"/>
-      <c r="G21" t="s" s="24">
-        <v>21</v>
-      </c>
-      <c r="H21" s="19"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
-    </row>
-    <row r="22" ht="17.25" customHeight="1">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-    </row>
-    <row r="23" ht="19.5" customHeight="1">
-      <c r="A23" s="20">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s" s="24">
-        <v>44</v>
-      </c>
-      <c r="C23" t="s" s="24">
-        <v>45</v>
-      </c>
-      <c r="D23" t="s" s="24">
-        <v>46</v>
-      </c>
-      <c r="E23" t="s" s="24">
-        <v>29</v>
-      </c>
-      <c r="F23" s="19"/>
-      <c r="G23" t="s" s="24">
-        <v>21</v>
-      </c>
-      <c r="H23" s="19"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-    </row>
-    <row r="24" ht="19.5" customHeight="1">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-    </row>
-    <row r="25" ht="21" customHeight="1">
-      <c r="A25" s="20">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s" s="24">
-        <v>47</v>
-      </c>
-      <c r="C25" t="s" s="24">
-        <v>48</v>
-      </c>
-      <c r="D25" t="s" s="24">
-        <v>49</v>
-      </c>
-      <c r="E25" t="s" s="24">
-        <v>20</v>
-      </c>
-      <c r="F25" s="19"/>
-      <c r="G25" t="s" s="24">
-        <v>21</v>
-      </c>
-      <c r="H25" s="19"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-    </row>
-    <row r="26" ht="30" customHeight="1">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-    </row>
-    <row r="27" ht="30" customHeight="1">
-      <c r="A27" s="20">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s" s="24">
-        <v>50</v>
-      </c>
-      <c r="C27" t="s" s="24">
-        <v>51</v>
-      </c>
-      <c r="D27" t="s" s="24">
-        <v>52</v>
-      </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="19"/>
-      <c r="G27" t="s" s="23">
-        <v>53</v>
-      </c>
-      <c r="H27" t="s" s="28">
-        <v>54</v>
-      </c>
-      <c r="I27" s="25"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
-    </row>
-    <row r="28" ht="30" customHeight="1">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-    </row>
-    <row r="29" ht="27" customHeight="1">
-      <c r="A29" s="20">
-        <v>4</v>
-      </c>
-      <c r="B29" t="s" s="24">
-        <v>55</v>
-      </c>
-      <c r="C29" t="s" s="29">
-        <v>56</v>
-      </c>
-      <c r="D29" t="s" s="24">
-        <v>57</v>
-      </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="19"/>
-      <c r="G29" t="s" s="23">
-        <v>58</v>
-      </c>
-      <c r="H29" t="s" s="28">
-        <v>59</v>
-      </c>
-      <c r="I29" s="25"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
-    </row>
-    <row r="30" ht="27" customHeight="1">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="22"/>
+      <c r="B30" t="s" s="34">
+        <v>65</v>
+      </c>
+      <c r="C30" t="s" s="42">
+        <v>66</v>
+      </c>
+      <c r="D30" t="s" s="33">
+        <v>67</v>
+      </c>
+      <c r="E30" s="36"/>
+      <c r="F30" s="20"/>
+      <c r="G30" t="s" s="24">
+        <v>63</v>
+      </c>
+      <c r="H30" t="s" s="37">
+        <v>68</v>
+      </c>
+      <c r="I30" s="38"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
     </row>
     <row r="31" ht="27" customHeight="1">
-      <c r="A31" s="20">
-        <v>2</v>
-      </c>
-      <c r="B31" t="s" s="24">
-        <v>60</v>
-      </c>
-      <c r="C31" t="s" s="29">
-        <v>61</v>
-      </c>
-      <c r="D31" t="s" s="24">
-        <v>62</v>
-      </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="19"/>
-      <c r="G31" t="s" s="23">
-        <v>58</v>
-      </c>
-      <c r="H31" t="s" s="28">
-        <v>63</v>
-      </c>
-      <c r="I31" s="25"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="22"/>
-    </row>
-    <row r="32" ht="27" customHeight="1">
-      <c r="A32" s="20"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="22"/>
-    </row>
-    <row r="33" ht="27" customHeight="1">
-      <c r="A33" s="20">
-        <v>1</v>
-      </c>
-      <c r="B33" t="s" s="24">
-        <v>64</v>
-      </c>
-      <c r="C33" t="s" s="24">
-        <v>65</v>
-      </c>
-      <c r="D33" t="s" s="24">
-        <v>66</v>
-      </c>
-      <c r="E33" s="20"/>
-      <c r="F33" s="19"/>
-      <c r="G33" t="s" s="23">
-        <v>67</v>
-      </c>
-      <c r="H33" t="s" s="28">
-        <v>68</v>
-      </c>
-      <c r="I33" s="25"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="22"/>
-    </row>
-    <row r="34" ht="27" customHeight="1">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="22"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="22"/>
-    </row>
-    <row r="35" ht="27" customHeight="1">
-      <c r="A35" s="20">
-        <v>2</v>
-      </c>
-      <c r="B35" t="s" s="24">
-        <v>69</v>
-      </c>
-      <c r="C35" t="s" s="24">
-        <v>70</v>
-      </c>
-      <c r="D35" t="s" s="24">
-        <v>71</v>
-      </c>
-      <c r="E35" s="20"/>
-      <c r="F35" s="19"/>
-      <c r="G35" t="s" s="23">
-        <v>67</v>
-      </c>
-      <c r="H35" t="s" s="23">
-        <v>72</v>
-      </c>
-      <c r="I35" s="25"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="22"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="22"/>
-      <c r="N35" s="22"/>
-    </row>
-    <row r="36" ht="27" customHeight="1">
-      <c r="A36" s="20"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="22"/>
-    </row>
-    <row r="37" ht="27" customHeight="1">
-      <c r="A37" s="20">
-        <v>2</v>
-      </c>
-      <c r="B37" t="s" s="24">
-        <v>73</v>
-      </c>
-      <c r="C37" t="s" s="24">
-        <v>74</v>
-      </c>
-      <c r="D37" t="s" s="24">
-        <v>75</v>
-      </c>
-      <c r="E37" s="20"/>
-      <c r="F37" s="19"/>
-      <c r="G37" t="s" s="23">
-        <v>58</v>
-      </c>
-      <c r="H37" t="s" s="23">
-        <v>76</v>
-      </c>
-      <c r="I37" s="25"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
-      <c r="N37" s="22"/>
-    </row>
-    <row r="38" ht="27" customHeight="1">
-      <c r="A38" s="20"/>
+      <c r="A31" s="43"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="23"/>
+      <c r="N31" s="23"/>
+    </row>
+    <row r="32" ht="30" customHeight="1">
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+    </row>
+    <row r="33" ht="30" customHeight="1">
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
+    </row>
+    <row r="34" ht="45" customHeight="1">
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="23"/>
+      <c r="N34" s="23"/>
+    </row>
+    <row r="35" ht="45" customHeight="1">
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="23"/>
+      <c r="N35" s="23"/>
+    </row>
+    <row r="36" ht="45" customHeight="1">
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="23"/>
+      <c r="M36" s="23"/>
+      <c r="N36" s="23"/>
+    </row>
+    <row r="37" ht="30" customHeight="1">
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="23"/>
+      <c r="L37" s="23"/>
+      <c r="M37" s="23"/>
+      <c r="N37" s="23"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="29"/>
       <c r="B38" s="20"/>
       <c r="C38" s="20"/>
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="21"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
       <c r="K38" s="22"/>
       <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
-      <c r="N38" s="22"/>
-    </row>
-    <row r="39" ht="27" customHeight="1">
-      <c r="A39" s="20">
-        <v>1</v>
-      </c>
-      <c r="B39" t="s" s="24">
-        <v>77</v>
-      </c>
-      <c r="C39" t="s" s="24">
-        <v>78</v>
-      </c>
+      <c r="M38" s="23"/>
+      <c r="N38" s="23"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" s="29"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
       <c r="D39" t="s" s="24">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="E39" s="20"/>
-      <c r="F39" s="19"/>
-      <c r="G39" t="s" s="23">
-        <v>80</v>
-      </c>
-      <c r="H39" t="s" s="23">
-        <v>81</v>
-      </c>
-      <c r="I39" s="25"/>
-      <c r="J39" s="21"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+      <c r="I39" s="20"/>
+      <c r="J39" s="20"/>
       <c r="K39" s="22"/>
       <c r="L39" s="22"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="22"/>
-    </row>
-    <row r="40" ht="27" customHeight="1">
-      <c r="A40" s="31"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="21"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="22"/>
-      <c r="N40" s="22"/>
-    </row>
-    <row r="41" ht="27" customHeight="1">
-      <c r="A41" s="32">
-        <v>2</v>
-      </c>
-      <c r="B41" t="s" s="33">
-        <v>82</v>
-      </c>
-      <c r="C41" t="s" s="34">
-        <v>83</v>
-      </c>
-      <c r="D41" t="s" s="32">
-        <v>84</v>
-      </c>
-      <c r="E41" s="35"/>
-      <c r="F41" s="19"/>
-      <c r="G41" t="s" s="23">
-        <v>85</v>
-      </c>
-      <c r="H41" t="s" s="36">
-        <v>86</v>
-      </c>
-      <c r="I41" s="37"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="22"/>
-      <c r="L41" s="22"/>
-      <c r="M41" s="22"/>
-      <c r="N41" s="22"/>
-    </row>
-    <row r="42" ht="27" customHeight="1">
-      <c r="A42" s="38"/>
-      <c r="B42" s="35"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="21"/>
-      <c r="K42" s="22"/>
-      <c r="L42" s="22"/>
-      <c r="M42" s="22"/>
-      <c r="N42" s="22"/>
-    </row>
-    <row r="43" ht="27" customHeight="1">
-      <c r="A43" s="32">
-        <v>1</v>
-      </c>
-      <c r="B43" t="s" s="33">
-        <v>87</v>
-      </c>
-      <c r="C43" t="s" s="41">
-        <v>88</v>
-      </c>
-      <c r="D43" t="s" s="32">
-        <v>89</v>
-      </c>
-      <c r="E43" s="35"/>
-      <c r="F43" s="19"/>
-      <c r="G43" t="s" s="23">
-        <v>85</v>
-      </c>
-      <c r="H43" t="s" s="36">
-        <v>90</v>
-      </c>
-      <c r="I43" s="37"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="22"/>
-      <c r="L43" s="22"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="22"/>
-    </row>
-    <row r="44" ht="27" customHeight="1">
-      <c r="A44" s="42"/>
-      <c r="B44" s="42"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="42"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="19"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="21"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="22"/>
-      <c r="M44" s="22"/>
-      <c r="N44" s="22"/>
-    </row>
-    <row r="45" ht="30" customHeight="1">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="21"/>
-      <c r="K45" s="22"/>
-      <c r="L45" s="22"/>
-      <c r="M45" s="22"/>
-      <c r="N45" s="22"/>
-    </row>
-    <row r="46" ht="30" customHeight="1">
-      <c r="A46" s="20"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="22"/>
-      <c r="N46" s="22"/>
-    </row>
-    <row r="47" ht="45" customHeight="1">
-      <c r="A47" s="20"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="19"/>
-      <c r="I47" s="27"/>
-      <c r="J47" s="21"/>
-      <c r="K47" s="22"/>
-      <c r="L47" s="22"/>
-      <c r="M47" s="22"/>
-      <c r="N47" s="22"/>
-    </row>
-    <row r="48" ht="45" customHeight="1">
-      <c r="A48" s="20"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
-      <c r="I48" s="27"/>
-      <c r="J48" s="21"/>
-      <c r="K48" s="22"/>
-      <c r="L48" s="22"/>
-      <c r="M48" s="22"/>
-      <c r="N48" s="22"/>
-    </row>
-    <row r="49" ht="45" customHeight="1">
-      <c r="A49" s="20"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
-      <c r="I49" s="27"/>
-      <c r="J49" s="21"/>
-      <c r="K49" s="22"/>
-      <c r="L49" s="22"/>
-      <c r="M49" s="22"/>
-      <c r="N49" s="22"/>
-    </row>
-    <row r="50" ht="30" customHeight="1">
-      <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="27"/>
-      <c r="J50" s="21"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="22"/>
-      <c r="M50" s="22"/>
-      <c r="N50" s="22"/>
-    </row>
-    <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="25"/>
-      <c r="B51" s="19"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="19"/>
-      <c r="I51" s="19"/>
-      <c r="J51" s="19"/>
-      <c r="K51" s="21"/>
-      <c r="L51" s="21"/>
-      <c r="M51" s="22"/>
-      <c r="N51" s="22"/>
-    </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="25"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
-      <c r="D52" t="s" s="23">
-        <v>91</v>
-      </c>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="19"/>
-      <c r="I52" s="19"/>
-      <c r="J52" s="19"/>
-      <c r="K52" s="21"/>
-      <c r="L52" s="21"/>
-      <c r="M52" s="22"/>
-      <c r="N52" s="22"/>
+      <c r="M39" s="23"/>
+      <c r="N39" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H27" r:id="rId1" location="" tooltip="" display=""/>
-    <hyperlink ref="H29" r:id="rId2" location="" tooltip="" display=""/>
-    <hyperlink ref="H31" r:id="rId3" location="" tooltip="" display=""/>
-    <hyperlink ref="H33" r:id="rId4" location="" tooltip="" display=""/>
-    <hyperlink ref="H35" r:id="rId5" location="" tooltip="" display=""/>
-    <hyperlink ref="H37" r:id="rId6" location="" tooltip="" display=""/>
-    <hyperlink ref="H39" r:id="rId7" location="" tooltip="" display=""/>
+    <hyperlink ref="H14" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="H16" r:id="rId2" location="" tooltip="" display=""/>
+    <hyperlink ref="H18" r:id="rId3" location="" tooltip="" display=""/>
+    <hyperlink ref="H20" r:id="rId4" location="" tooltip="" display=""/>
+    <hyperlink ref="H22" r:id="rId5" location="" tooltip="" display=""/>
+    <hyperlink ref="H24" r:id="rId6" location="" tooltip="" display=""/>
+    <hyperlink ref="H26" r:id="rId7" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>